<commit_message>
Lambda function get and insert into AWS RDS, update Work Credit excel
</commit_message>
<xml_diff>
--- a/Huy/WorkCredit.xlsx
+++ b/Huy/WorkCredit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hvuongbaovo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Intern-Repo\Huy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9F639D4-7F8B-4A56-A0E9-BE694D88DC0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8636F5A5-2A61-4997-B4FC-C6F7E1A8B389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Date</t>
   </si>
@@ -251,6 +251,67 @@
   <si>
     <t>* Nguyên nhân do nhiều người truy cập cùng 1 lúc =&gt; cách solve: xóa và tái khởi động docker container: docker compose down, docker compose up -d</t>
   </si>
+  <si>
+    <t>* Relabel dataset để train model (task này k liên quan đến cty)</t>
+  </si>
+  <si>
+    <t>13/5/2025</t>
+  </si>
+  <si>
+    <t>14/5/2025</t>
+  </si>
+  <si>
+    <t>15/5/2025</t>
+  </si>
+  <si>
+    <t>16/5/2025</t>
+  </si>
+  <si>
+    <t>* Self study về AWS Lambda, AWS Aurora và RDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Biết dc cách config Aurora và RDS. Tuy nhiên Aurora không bao gồm trong free tier. 
+* Biết được cách viết code cho Lambda Function: def lambda_handler(event, context).
+</t>
+  </si>
+  <si>
+    <t>* Demo code trên Lambda và kết hợp ứng dụng vs AWS Aurora để truy vấn và insert dữ liệu</t>
+  </si>
+  <si>
+    <t>* Present cho team về AWS Aurora và RDS.
+* So sánh ưu và nhược điểm của Aurora và các AWS RDS khác.</t>
+  </si>
+  <si>
+    <t>* Hãy present nhánh hơn, dùng giấy note lại những j sẽ nói trên slide để tránh quên content</t>
+  </si>
+  <si>
+    <t>* Viết code Lambda function để tương tác với AWS RDS</t>
+  </si>
+  <si>
+    <t>* Code chạy trên local thành công lấy được dữ liệu và insert dữ liệu thành công vào AWS MySQL.
+* Tuy nhiên khi deploy lên AWS Lambda Function thì bị lỗi không connect dc vs RDS.</t>
+  </si>
+  <si>
+    <t>* Check lại thử phần Configuration VPC</t>
+  </si>
+  <si>
+    <t>19/5/2025</t>
+  </si>
+  <si>
+    <t>* Tìm cách implement lại Lambda function để tương tác vs AWS RDS và kết hợp vs API Gateway của Khoa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Fix được lỗi, connect thành công tới AWS RDS.
+* Test thử thành công API Get, thành công lấy dc tất cả record từ RDS để in ra trên console của PostMan.
+* Test thử thành công API Post, thành công insert record vào trong RDS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Mục configuration phần connect to RDS , nhấn vào connect to RDS để tạo connection thì sẽ chạy dc code bên Lambda.
+</t>
+  </si>
+  <si>
+    <t>* Thử lấy dữ liệu từ S3</t>
+  </si>
 </sst>
 </file>
 
@@ -304,7 +365,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -323,6 +384,9 @@
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -605,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AL512"/>
+  <dimension ref="A1:AL510"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2070,11 +2134,13 @@
       <c r="AL33" s="1"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
+      <c r="A34" s="5">
+        <v>45996</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -2109,12 +2175,14 @@
       <c r="AK34" s="1"/>
       <c r="AL34" s="1"/>
     </row>
-    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
+    <row r="35" spans="1:38" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
@@ -2150,11 +2218,13 @@
       <c r="AL35" s="1"/>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
+      <c r="A36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -2190,11 +2260,11 @@
       <c r="AL36" s="1"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
@@ -2230,11 +2300,13 @@
       <c r="AL37" s="1"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
+      <c r="A38" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
@@ -2269,12 +2341,18 @@
       <c r="AK38" s="1"/>
       <c r="AL38" s="1"/>
     </row>
-    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
+    <row r="39" spans="1:38" ht="105" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
@@ -2310,11 +2388,12 @@
       <c r="AL39" s="1"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
+      <c r="A40" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
@@ -2349,12 +2428,16 @@
       <c r="AK40" s="1"/>
       <c r="AL40" s="1"/>
     </row>
-    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
+    <row r="41" spans="1:38" ht="60" x14ac:dyDescent="0.25">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E41" s="2"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
@@ -2390,11 +2473,12 @@
       <c r="AL41" s="1"/>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+      <c r="A42" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
@@ -2429,12 +2513,18 @@
       <c r="AK42" s="1"/>
       <c r="AL42" s="1"/>
     </row>
-    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
+    <row r="43" spans="1:38" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
@@ -2470,11 +2560,13 @@
       <c r="AL43" s="1"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
+      <c r="A44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
@@ -2509,12 +2601,20 @@
       <c r="AK44" s="1"/>
       <c r="AL44" s="1"/>
     </row>
-    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
+    <row r="45" spans="1:38" ht="120" x14ac:dyDescent="0.25">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2550,11 +2650,11 @@
       <c r="AL45" s="1"/>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
@@ -2590,11 +2690,11 @@
       <c r="AL46" s="1"/>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
@@ -2630,11 +2730,11 @@
       <c r="AL47" s="1"/>
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
@@ -2670,11 +2770,11 @@
       <c r="AL48" s="1"/>
     </row>
     <row r="49" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
@@ -2710,11 +2810,11 @@
       <c r="AL49" s="1"/>
     </row>
     <row r="50" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
@@ -2750,11 +2850,11 @@
       <c r="AL50" s="1"/>
     </row>
     <row r="51" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
@@ -2790,11 +2890,11 @@
       <c r="AL51" s="1"/>
     </row>
     <row r="52" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
@@ -2830,11 +2930,11 @@
       <c r="AL52" s="1"/>
     </row>
     <row r="53" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -2870,11 +2970,11 @@
       <c r="AL53" s="1"/>
     </row>
     <row r="54" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2910,11 +3010,11 @@
       <c r="AL54" s="1"/>
     </row>
     <row r="55" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -2950,11 +3050,11 @@
       <c r="AL55" s="1"/>
     </row>
     <row r="56" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -2990,11 +3090,11 @@
       <c r="AL56" s="1"/>
     </row>
     <row r="57" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
@@ -3030,11 +3130,11 @@
       <c r="AL57" s="1"/>
     </row>
     <row r="58" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
@@ -3070,11 +3170,11 @@
       <c r="AL58" s="1"/>
     </row>
     <row r="59" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
@@ -3110,11 +3210,11 @@
       <c r="AL59" s="1"/>
     </row>
     <row r="60" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
@@ -3150,11 +3250,11 @@
       <c r="AL60" s="1"/>
     </row>
     <row r="61" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
@@ -3190,11 +3290,11 @@
       <c r="AL61" s="1"/>
     </row>
     <row r="62" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
@@ -3230,11 +3330,11 @@
       <c r="AL62" s="1"/>
     </row>
     <row r="63" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
@@ -3270,11 +3370,11 @@
       <c r="AL63" s="1"/>
     </row>
     <row r="64" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
@@ -3310,11 +3410,11 @@
       <c r="AL64" s="1"/>
     </row>
     <row r="65" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
@@ -3350,11 +3450,11 @@
       <c r="AL65" s="1"/>
     </row>
     <row r="66" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
@@ -3390,11 +3490,11 @@
       <c r="AL66" s="1"/>
     </row>
     <row r="67" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
@@ -3430,11 +3530,11 @@
       <c r="AL67" s="1"/>
     </row>
     <row r="68" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
@@ -3470,11 +3570,11 @@
       <c r="AL68" s="1"/>
     </row>
     <row r="69" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
+      <c r="A69" s="2"/>
+      <c r="B69" s="2"/>
+      <c r="C69" s="2"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="2"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
@@ -3510,11 +3610,11 @@
       <c r="AL69" s="1"/>
     </row>
     <row r="70" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+      <c r="E70" s="2"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
@@ -3550,11 +3650,11 @@
       <c r="AL70" s="1"/>
     </row>
     <row r="71" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
+      <c r="A71" s="2"/>
+      <c r="B71" s="2"/>
+      <c r="C71" s="2"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
@@ -3590,11 +3690,11 @@
       <c r="AL71" s="1"/>
     </row>
     <row r="72" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
+      <c r="A72" s="2"/>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
@@ -3630,11 +3730,11 @@
       <c r="AL72" s="1"/>
     </row>
     <row r="73" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
@@ -3670,11 +3770,11 @@
       <c r="AL73" s="1"/>
     </row>
     <row r="74" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
+      <c r="A74" s="2"/>
+      <c r="B74" s="2"/>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
@@ -3710,11 +3810,11 @@
       <c r="AL74" s="1"/>
     </row>
     <row r="75" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
+      <c r="A75" s="2"/>
+      <c r="B75" s="2"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
@@ -3750,11 +3850,11 @@
       <c r="AL75" s="1"/>
     </row>
     <row r="76" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
+      <c r="A76" s="2"/>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
@@ -3790,11 +3890,11 @@
       <c r="AL76" s="1"/>
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
+      <c r="A77" s="2"/>
+      <c r="B77" s="2"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
@@ -21149,86 +21249,6 @@
       <c r="AK510" s="1"/>
       <c r="AL510" s="1"/>
     </row>
-    <row r="511" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A511" s="1"/>
-      <c r="B511" s="1"/>
-      <c r="C511" s="1"/>
-      <c r="D511" s="1"/>
-      <c r="E511" s="1"/>
-      <c r="F511" s="1"/>
-      <c r="G511" s="1"/>
-      <c r="H511" s="1"/>
-      <c r="I511" s="1"/>
-      <c r="J511" s="1"/>
-      <c r="K511" s="1"/>
-      <c r="L511" s="1"/>
-      <c r="M511" s="1"/>
-      <c r="N511" s="1"/>
-      <c r="O511" s="1"/>
-      <c r="P511" s="1"/>
-      <c r="Q511" s="1"/>
-      <c r="R511" s="1"/>
-      <c r="S511" s="1"/>
-      <c r="T511" s="1"/>
-      <c r="U511" s="1"/>
-      <c r="V511" s="1"/>
-      <c r="W511" s="1"/>
-      <c r="X511" s="1"/>
-      <c r="Y511" s="1"/>
-      <c r="Z511" s="1"/>
-      <c r="AA511" s="1"/>
-      <c r="AB511" s="1"/>
-      <c r="AC511" s="1"/>
-      <c r="AD511" s="1"/>
-      <c r="AE511" s="1"/>
-      <c r="AF511" s="1"/>
-      <c r="AG511" s="1"/>
-      <c r="AH511" s="1"/>
-      <c r="AI511" s="1"/>
-      <c r="AJ511" s="1"/>
-      <c r="AK511" s="1"/>
-      <c r="AL511" s="1"/>
-    </row>
-    <row r="512" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A512" s="1"/>
-      <c r="B512" s="1"/>
-      <c r="C512" s="1"/>
-      <c r="D512" s="1"/>
-      <c r="E512" s="1"/>
-      <c r="F512" s="1"/>
-      <c r="G512" s="1"/>
-      <c r="H512" s="1"/>
-      <c r="I512" s="1"/>
-      <c r="J512" s="1"/>
-      <c r="K512" s="1"/>
-      <c r="L512" s="1"/>
-      <c r="M512" s="1"/>
-      <c r="N512" s="1"/>
-      <c r="O512" s="1"/>
-      <c r="P512" s="1"/>
-      <c r="Q512" s="1"/>
-      <c r="R512" s="1"/>
-      <c r="S512" s="1"/>
-      <c r="T512" s="1"/>
-      <c r="U512" s="1"/>
-      <c r="V512" s="1"/>
-      <c r="W512" s="1"/>
-      <c r="X512" s="1"/>
-      <c r="Y512" s="1"/>
-      <c r="Z512" s="1"/>
-      <c r="AA512" s="1"/>
-      <c r="AB512" s="1"/>
-      <c r="AC512" s="1"/>
-      <c r="AD512" s="1"/>
-      <c r="AE512" s="1"/>
-      <c r="AF512" s="1"/>
-      <c r="AG512" s="1"/>
-      <c r="AH512" s="1"/>
-      <c r="AI512" s="1"/>
-      <c r="AJ512" s="1"/>
-      <c r="AK512" s="1"/>
-      <c r="AL512" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>